<commit_message>
cube file calculation 修正
</commit_message>
<xml_diff>
--- a/arranged_dataset/DIP-chloride.xlsx
+++ b/arranged_dataset/DIP-chloride.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>smiles</t>
   </si>
@@ -112,6 +112,12 @@
     <t>FNENWZWNOPCZGK-UHFFFAOYSA-N</t>
   </si>
   <si>
+    <t>BrCC(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>LIGACIXOYTUXAW-UHFFFAOYSA-N</t>
+  </si>
+  <si>
     <t>c1cc(Br)ccc1C(=O)C</t>
   </si>
   <si>
@@ -130,6 +136,12 @@
     <t>ADCYRBXQAJXJTD-UHFFFAOYSA-N</t>
   </si>
   <si>
+    <t>ClCC(=O)c1c(Cl)cc(Cl)cc1</t>
+  </si>
+  <si>
+    <t>VYWPPRLJNVHPEU-UHFFFAOYSA-N</t>
+  </si>
+  <si>
     <t>c1cc(Br)ccc1c2cc(Cl)ccc2C(=O)CCC</t>
   </si>
   <si>
@@ -220,6 +232,48 @@
     <t>IQZLUWLMQNGTIW-UHFFFAOYSA-N</t>
   </si>
   <si>
+    <t>Oc1ccccc1C(=O)C</t>
+  </si>
+  <si>
+    <t>JECYUBVRTQDVAT-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>Oc1cccc(OC)c1C(=O)C</t>
+  </si>
+  <si>
+    <t>UENLHUMCIOWYQN-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>Oc1ccc(OC)cc1C(=O)C</t>
+  </si>
+  <si>
+    <t>MLIBGOFSXXWRIY-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>Oc1ccc(C)cc1C(=O)C</t>
+  </si>
+  <si>
+    <t>YNPDFBFVMJNGKZ-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>Oc1ccc(F)cc1C(=O)C</t>
+  </si>
+  <si>
+    <t>KOFFXZYMDLWRHX-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>Oc1c(Cl)cc(Cl)cc1C(=O)C</t>
+  </si>
+  <si>
+    <t>CJFYGRLJDKWMDI-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>Oc1cc(OC)cc(C(=O)OC)c1C(=O)C</t>
+  </si>
+  <si>
+    <t>WRYKPYJMRHQDBM-UHFFFAOYSA-N</t>
+  </si>
+  <si>
     <t>COc1cccc(OC)c1C(=O)C</t>
   </si>
   <si>
@@ -268,6 +322,36 @@
     <t>HXAOUYGZEOZTJO-UHFFFAOYSA-N</t>
   </si>
   <si>
+    <t>ClC(Cl)C(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>CERJZAHSUZVMCH-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>ClC(Cl)(Cl)C(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>OAMHTTBNEJBIKA-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>ClCC(=O)C</t>
+  </si>
+  <si>
+    <t>BULLHNJGPPOUOX-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>ClC(Cl)C(=O)C</t>
+  </si>
+  <si>
+    <t>CSVFWMMPUJDVKH-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>ClC(Cl)(Cl)C(=O)C</t>
+  </si>
+  <si>
+    <t>SMZHKGXSEAGRTI-UHFFFAOYSA-N</t>
+  </si>
+  <si>
     <t>COCC(=O)c1ccccc1</t>
   </si>
   <si>
@@ -380,6 +464,12 @@
   </si>
   <si>
     <t>KWOLFJPFCHCOCG-UHFFFAOYSA-N</t>
+  </si>
+  <si>
+    <t>ClCC(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>IMACFCSSMIZSPP-UHFFFAOYSA-N</t>
   </si>
   <si>
     <t>c1ccccc1/C=C/C(=O)C</t>
@@ -3019,6 +3109,576 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="83800950"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 68" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="85067775"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 69" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="86334600"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 70" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="87601425"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="88868250"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="90135075"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="91401900"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId74"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="92668725"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId75"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="93935550"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Picture 76" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId76"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="95202375"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId77"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="96469200"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Picture 78" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId78"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="97736025"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="80" name="Picture 79" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId79"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="99002850"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Picture 80" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId80"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="100269675"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Picture 81" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId81"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="101536500"/>
+          <a:ext cx="952500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="Picture 82" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId82"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="102803325"/>
           <a:ext cx="952500" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3316,7 +3976,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3574,13 +4234,13 @@
         <v>33</v>
       </c>
       <c r="D15">
-        <v>98.5</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>0.49352</v>
       </c>
       <c r="F15">
-        <v>-2.065179567503288</v>
+        <v>1.276582925099217</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="100" customHeight="1">
@@ -3608,13 +4268,13 @@
         <v>37</v>
       </c>
       <c r="D17">
-        <v>99</v>
+        <v>98.5</v>
       </c>
       <c r="E17">
         <v>0.49352</v>
       </c>
       <c r="F17">
-        <v>-2.26778354843842</v>
+        <v>-2.065179567503288</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="100" customHeight="1">
@@ -3642,13 +4302,13 @@
         <v>41</v>
       </c>
       <c r="D19">
-        <v>63</v>
+        <v>3.5</v>
       </c>
       <c r="E19">
         <v>0.49352</v>
       </c>
       <c r="F19">
-        <v>-0.2626596419205717</v>
+        <v>1.636897285266561</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="100" customHeight="1">
@@ -3659,13 +4319,13 @@
         <v>43</v>
       </c>
       <c r="D20">
-        <v>61.5</v>
+        <v>99</v>
       </c>
       <c r="E20">
         <v>0.49352</v>
       </c>
       <c r="F20">
-        <v>-0.2311543712701655</v>
+        <v>-2.26778354843842</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="100" customHeight="1">
@@ -3676,13 +4336,13 @@
         <v>45</v>
       </c>
       <c r="D21">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E21">
         <v>0.49352</v>
       </c>
       <c r="F21">
-        <v>-0.3948748769913301</v>
+        <v>-0.2626596419205717</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="100" customHeight="1">
@@ -3693,13 +4353,13 @@
         <v>47</v>
       </c>
       <c r="D22">
-        <v>72.5</v>
+        <v>61.5</v>
       </c>
       <c r="E22">
         <v>0.49352</v>
       </c>
       <c r="F22">
-        <v>-0.4784185629834727</v>
+        <v>-0.2311543712701655</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="100" customHeight="1">
@@ -3710,13 +4370,13 @@
         <v>49</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="E23">
-        <v>0.38805</v>
+        <v>0.49352</v>
       </c>
       <c r="F23">
-        <v>1.23324378886652</v>
+        <v>-0.3948748769913301</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="100" customHeight="1">
@@ -3727,13 +4387,13 @@
         <v>51</v>
       </c>
       <c r="D24">
-        <v>5.5</v>
+        <v>72.5</v>
       </c>
       <c r="E24">
-        <v>0.38805</v>
+        <v>0.49352</v>
       </c>
       <c r="F24">
-        <v>1.103556668584487</v>
+        <v>-0.4784185629834727</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="100" customHeight="1">
@@ -3744,13 +4404,13 @@
         <v>53</v>
       </c>
       <c r="D25">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>0.38805</v>
       </c>
       <c r="F25">
-        <v>-0.8978060342685433</v>
+        <v>1.23324378886652</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="100" customHeight="1">
@@ -3761,13 +4421,13 @@
         <v>55</v>
       </c>
       <c r="D26">
-        <v>99.5</v>
+        <v>5.5</v>
       </c>
       <c r="E26">
-        <v>0.49352</v>
+        <v>0.38805</v>
       </c>
       <c r="F26">
-        <v>-2.61235179709804</v>
+        <v>1.103556668584487</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="100" customHeight="1">
@@ -3778,13 +4438,13 @@
         <v>57</v>
       </c>
       <c r="D27">
-        <v>36.5</v>
+        <v>91</v>
       </c>
       <c r="E27">
-        <v>0.49352</v>
+        <v>0.38805</v>
       </c>
       <c r="F27">
-        <v>0.2732756675134899</v>
+        <v>-0.8978060342685433</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="100" customHeight="1">
@@ -3795,13 +4455,13 @@
         <v>59</v>
       </c>
       <c r="D28">
-        <v>99</v>
+        <v>99.5</v>
       </c>
       <c r="E28">
         <v>0.49352</v>
       </c>
       <c r="F28">
-        <v>-2.26778354843842</v>
+        <v>-2.61235179709804</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="100" customHeight="1">
@@ -3812,13 +4472,13 @@
         <v>61</v>
       </c>
       <c r="D29">
-        <v>98.5</v>
+        <v>36.5</v>
       </c>
       <c r="E29">
         <v>0.49352</v>
       </c>
       <c r="F29">
-        <v>-2.065179567503288</v>
+        <v>0.2732756675134899</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="100" customHeight="1">
@@ -3829,13 +4489,13 @@
         <v>63</v>
       </c>
       <c r="D30">
-        <v>97.5</v>
+        <v>99</v>
       </c>
       <c r="E30">
         <v>0.49352</v>
       </c>
       <c r="F30">
-        <v>-1.808040943597905</v>
+        <v>-2.26778354843842</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="100" customHeight="1">
@@ -3846,13 +4506,13 @@
         <v>65</v>
       </c>
       <c r="D31">
-        <v>93.5</v>
+        <v>98.5</v>
       </c>
       <c r="E31">
         <v>0.49352</v>
       </c>
       <c r="F31">
-        <v>-1.315802917695658</v>
+        <v>-2.065179567503288</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="100" customHeight="1">
@@ -3863,13 +4523,13 @@
         <v>67</v>
       </c>
       <c r="D32">
-        <v>97</v>
+        <v>97.5</v>
       </c>
       <c r="E32">
         <v>0.49352</v>
       </c>
       <c r="F32">
-        <v>-1.715524225407506</v>
+        <v>-1.808040943597905</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="100" customHeight="1">
@@ -3880,13 +4540,13 @@
         <v>69</v>
       </c>
       <c r="D33">
-        <v>40</v>
+        <v>93.5</v>
       </c>
       <c r="E33">
         <v>0.49352</v>
       </c>
       <c r="F33">
-        <v>0.2001051401535413</v>
+        <v>-1.315802917695658</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="100" customHeight="1">
@@ -3897,13 +4557,13 @@
         <v>71</v>
       </c>
       <c r="D34">
-        <v>96.5</v>
+        <v>97</v>
       </c>
       <c r="E34">
-        <v>0.54327</v>
+        <v>0.49352</v>
       </c>
       <c r="F34">
-        <v>-1.801907092249079</v>
+        <v>-1.715524225407506</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="100" customHeight="1">
@@ -3914,13 +4574,13 @@
         <v>73</v>
       </c>
       <c r="D35">
-        <v>97.5</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F35">
-        <v>-1.808040943597905</v>
+        <v>1.716814035582576</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="100" customHeight="1">
@@ -3931,13 +4591,13 @@
         <v>75</v>
       </c>
       <c r="D36">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F36">
-        <v>-1.715524225407506</v>
+        <v>2.269203661219363</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="100" customHeight="1">
@@ -3948,13 +4608,13 @@
         <v>77</v>
       </c>
       <c r="D37">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="E37">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F37">
-        <v>-1.715524225407506</v>
+        <v>1.34901111815735</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="100" customHeight="1">
@@ -3965,13 +4625,13 @@
         <v>79</v>
       </c>
       <c r="D38">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E38">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F38">
-        <v>-0.2001051401535412</v>
+        <v>1.34901111815735</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="100" customHeight="1">
@@ -3982,13 +4642,13 @@
         <v>81</v>
       </c>
       <c r="D39">
-        <v>98</v>
+        <v>10.5</v>
       </c>
       <c r="E39">
         <v>0.58307</v>
       </c>
       <c r="F39">
-        <v>-2.269203661219362</v>
+        <v>1.249439344048173</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="100" customHeight="1">
@@ -3999,13 +4659,13 @@
         <v>83</v>
       </c>
       <c r="D40">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="E40">
-        <v>0.49352</v>
+        <v>0.54327</v>
       </c>
       <c r="F40">
-        <v>-2.26778354843842</v>
+        <v>1.135836915731209</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="100" customHeight="1">
@@ -4016,13 +4676,13 @@
         <v>85</v>
       </c>
       <c r="D41">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="E41">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F41">
-        <v>1.808040943597903</v>
+        <v>1.716814035582576</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="100" customHeight="1">
@@ -4033,13 +4693,13 @@
         <v>87</v>
       </c>
       <c r="D42">
-        <v>98.5</v>
+        <v>40</v>
       </c>
       <c r="E42">
         <v>0.49352</v>
       </c>
       <c r="F42">
-        <v>-2.065179567503288</v>
+        <v>0.2001051401535413</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="100" customHeight="1">
@@ -4050,13 +4710,13 @@
         <v>89</v>
       </c>
       <c r="D43">
-        <v>99.5</v>
+        <v>96.5</v>
       </c>
       <c r="E43">
-        <v>0.49352</v>
+        <v>0.54327</v>
       </c>
       <c r="F43">
-        <v>-2.61235179709804</v>
+        <v>-1.801907092249079</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="100" customHeight="1">
@@ -4067,13 +4727,13 @@
         <v>91</v>
       </c>
       <c r="D44">
-        <v>99</v>
+        <v>97.5</v>
       </c>
       <c r="E44">
         <v>0.49352</v>
       </c>
       <c r="F44">
-        <v>-2.26778354843842</v>
+        <v>-1.808040943597905</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="100" customHeight="1">
@@ -4084,13 +4744,13 @@
         <v>93</v>
       </c>
       <c r="D45">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E45">
         <v>0.49352</v>
       </c>
       <c r="F45">
-        <v>-1.920691153523556</v>
+        <v>-1.715524225407506</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="100" customHeight="1">
@@ -4101,13 +4761,13 @@
         <v>95</v>
       </c>
       <c r="D46">
-        <v>97.5</v>
+        <v>97</v>
       </c>
       <c r="E46">
         <v>0.49352</v>
       </c>
       <c r="F46">
-        <v>-1.808040943597905</v>
+        <v>-1.715524225407506</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="100" customHeight="1">
@@ -4118,13 +4778,13 @@
         <v>97</v>
       </c>
       <c r="D47">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="E47">
         <v>0.49352</v>
       </c>
       <c r="F47">
-        <v>-1.141825110249225</v>
+        <v>-0.2001051401535412</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="100" customHeight="1">
@@ -4135,13 +4795,13 @@
         <v>99</v>
       </c>
       <c r="D48">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F48">
-        <v>-2.26778354843842</v>
+        <v>-2.269203661219362</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="100" customHeight="1">
@@ -4152,13 +4812,13 @@
         <v>101</v>
       </c>
       <c r="D49">
-        <v>96.5</v>
+        <v>99</v>
       </c>
       <c r="E49">
         <v>0.49352</v>
       </c>
       <c r="F49">
-        <v>-1.636897285266562</v>
+        <v>-2.26778354843842</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="100" customHeight="1">
@@ -4169,13 +4829,13 @@
         <v>103</v>
       </c>
       <c r="D50">
-        <v>95.5</v>
+        <v>9</v>
       </c>
       <c r="E50">
         <v>0.49352</v>
       </c>
       <c r="F50">
-        <v>-1.507727708802602</v>
+        <v>1.141825110249225</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="100" customHeight="1">
@@ -4186,13 +4846,13 @@
         <v>105</v>
       </c>
       <c r="D51">
-        <v>97.5</v>
+        <v>95.5</v>
       </c>
       <c r="E51">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F51">
-        <v>-1.808040943597905</v>
+        <v>-1.781307333383719</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="100" customHeight="1">
@@ -4203,13 +4863,13 @@
         <v>107</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E52">
         <v>0.49352</v>
       </c>
       <c r="F52">
-        <v>2.267783548438423</v>
+        <v>0.1796241929564407</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="100" customHeight="1">
@@ -4220,13 +4880,13 @@
         <v>109</v>
       </c>
       <c r="D53">
-        <v>98.5</v>
+        <v>42.5</v>
       </c>
       <c r="E53">
         <v>0.49352</v>
       </c>
       <c r="F53">
-        <v>-2.065179567503288</v>
+        <v>0.1491816558867302</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="100" customHeight="1">
@@ -4237,13 +4897,13 @@
         <v>111</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>95.5</v>
       </c>
       <c r="E54">
-        <v>0.49352</v>
+        <v>0.58307</v>
       </c>
       <c r="F54">
-        <v>1.920691153523556</v>
+        <v>-1.781307333383719</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="100" customHeight="1">
@@ -4254,13 +4914,13 @@
         <v>113</v>
       </c>
       <c r="D55">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="E55">
         <v>0.49352</v>
       </c>
       <c r="F55">
-        <v>2.612351797098031</v>
+        <v>1.808040943597903</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="100" customHeight="1">
@@ -4271,13 +4931,13 @@
         <v>115</v>
       </c>
       <c r="D56">
-        <v>0.5</v>
+        <v>98.5</v>
       </c>
       <c r="E56">
         <v>0.49352</v>
       </c>
       <c r="F56">
-        <v>2.612351797098031</v>
+        <v>-2.065179567503288</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="100" customHeight="1">
@@ -4288,13 +4948,13 @@
         <v>117</v>
       </c>
       <c r="D57">
-        <v>0.5</v>
+        <v>99.5</v>
       </c>
       <c r="E57">
         <v>0.49352</v>
       </c>
       <c r="F57">
-        <v>2.612351797098031</v>
+        <v>-2.61235179709804</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="100" customHeight="1">
@@ -4305,13 +4965,13 @@
         <v>119</v>
       </c>
       <c r="D58">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="E58">
         <v>0.49352</v>
       </c>
       <c r="F58">
-        <v>-0.3273489621763136</v>
+        <v>-2.26778354843842</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="100" customHeight="1">
@@ -4322,13 +4982,13 @@
         <v>121</v>
       </c>
       <c r="D59">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E59">
         <v>0.49352</v>
       </c>
       <c r="F59">
-        <v>-2.26778354843842</v>
+        <v>-1.920691153523556</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="100" customHeight="1">
@@ -4339,13 +4999,13 @@
         <v>123</v>
       </c>
       <c r="D60">
-        <v>90.5</v>
+        <v>97.5</v>
       </c>
       <c r="E60">
         <v>0.49352</v>
       </c>
       <c r="F60">
-        <v>-1.112422729872088</v>
+        <v>-1.808040943597905</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="100" customHeight="1">
@@ -4356,13 +5016,13 @@
         <v>125</v>
       </c>
       <c r="D61">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="E61">
         <v>0.49352</v>
       </c>
       <c r="F61">
-        <v>-0.3720014599087911</v>
+        <v>-1.141825110249225</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="100" customHeight="1">
@@ -4373,13 +5033,13 @@
         <v>127</v>
       </c>
       <c r="D62">
-        <v>39.5</v>
+        <v>99</v>
       </c>
       <c r="E62">
         <v>0.49352</v>
       </c>
       <c r="F62">
-        <v>0.2104086459133793</v>
+        <v>-2.26778354843842</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="100" customHeight="1">
@@ -4390,13 +5050,13 @@
         <v>129</v>
       </c>
       <c r="D63">
-        <v>41.5</v>
+        <v>96.5</v>
       </c>
       <c r="E63">
         <v>0.49352</v>
       </c>
       <c r="F63">
-        <v>0.1694418635416117</v>
+        <v>-1.636897285266562</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="100" customHeight="1">
@@ -4407,13 +5067,13 @@
         <v>131</v>
       </c>
       <c r="D64">
-        <v>36</v>
+        <v>95.5</v>
       </c>
       <c r="E64">
         <v>0.49352</v>
       </c>
       <c r="F64">
-        <v>0.2839537127928058</v>
+        <v>-1.507727708802602</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="100" customHeight="1">
@@ -4424,13 +5084,13 @@
         <v>133</v>
       </c>
       <c r="D65">
-        <v>23.5</v>
+        <v>97.5</v>
       </c>
       <c r="E65">
         <v>0.49352</v>
       </c>
       <c r="F65">
-        <v>0.5824968785696466</v>
+        <v>-1.808040943597905</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="100" customHeight="1">
@@ -4444,10 +5104,10 @@
         <v>1</v>
       </c>
       <c r="E66">
-        <v>0.58904</v>
+        <v>0.49352</v>
       </c>
       <c r="F66">
-        <v>2.706709396523279</v>
+        <v>2.267783548438423</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="100" customHeight="1">
@@ -4458,13 +5118,13 @@
         <v>137</v>
       </c>
       <c r="D67">
-        <v>30.5</v>
+        <v>98.5</v>
       </c>
       <c r="E67">
         <v>0.49352</v>
       </c>
       <c r="F67">
-        <v>0.4064631060318465</v>
+        <v>-2.065179567503288</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="100" customHeight="1">
@@ -4475,12 +5135,267 @@
         <v>139</v>
       </c>
       <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>0.49352</v>
+      </c>
+      <c r="F68">
+        <v>1.920691153523556</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="100" customHeight="1">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69">
+        <v>0.5</v>
+      </c>
+      <c r="E69">
+        <v>0.49352</v>
+      </c>
+      <c r="F69">
+        <v>2.612351797098031</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="100" customHeight="1">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" t="s">
+        <v>143</v>
+      </c>
+      <c r="D70">
+        <v>0.5</v>
+      </c>
+      <c r="E70">
+        <v>0.49352</v>
+      </c>
+      <c r="F70">
+        <v>2.612351797098031</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="100" customHeight="1">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D71">
+        <v>0.5</v>
+      </c>
+      <c r="E71">
+        <v>0.49352</v>
+      </c>
+      <c r="F71">
+        <v>2.612351797098031</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="100" customHeight="1">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72">
+        <v>66</v>
+      </c>
+      <c r="E72">
+        <v>0.49352</v>
+      </c>
+      <c r="F72">
+        <v>-0.3273489621763136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="100" customHeight="1">
+      <c r="A73" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" t="s">
+        <v>149</v>
+      </c>
+      <c r="D73">
+        <v>99</v>
+      </c>
+      <c r="E73">
+        <v>0.49352</v>
+      </c>
+      <c r="F73">
+        <v>-2.26778354843842</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="100" customHeight="1">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74">
+        <v>2.5</v>
+      </c>
+      <c r="E74">
+        <v>0.49352</v>
+      </c>
+      <c r="F74">
+        <v>1.808040943597903</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="100" customHeight="1">
+      <c r="A75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" t="s">
+        <v>153</v>
+      </c>
+      <c r="D75">
+        <v>90.5</v>
+      </c>
+      <c r="E75">
+        <v>0.49352</v>
+      </c>
+      <c r="F75">
+        <v>-1.112422729872088</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="100" customHeight="1">
+      <c r="A76" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76">
+        <v>68</v>
+      </c>
+      <c r="E76">
+        <v>0.49352</v>
+      </c>
+      <c r="F76">
+        <v>-0.3720014599087911</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="100" customHeight="1">
+      <c r="A77" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77">
+        <v>39.5</v>
+      </c>
+      <c r="E77">
+        <v>0.49352</v>
+      </c>
+      <c r="F77">
+        <v>0.2104086459133793</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="100" customHeight="1">
+      <c r="A78" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" t="s">
+        <v>159</v>
+      </c>
+      <c r="D78">
+        <v>41.5</v>
+      </c>
+      <c r="E78">
+        <v>0.49352</v>
+      </c>
+      <c r="F78">
+        <v>0.1694418635416117</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="100" customHeight="1">
+      <c r="A79" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" t="s">
+        <v>161</v>
+      </c>
+      <c r="D79">
+        <v>36</v>
+      </c>
+      <c r="E79">
+        <v>0.49352</v>
+      </c>
+      <c r="F79">
+        <v>0.2839537127928058</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="100" customHeight="1">
+      <c r="A80" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" t="s">
+        <v>163</v>
+      </c>
+      <c r="D80">
+        <v>23.5</v>
+      </c>
+      <c r="E80">
+        <v>0.49352</v>
+      </c>
+      <c r="F80">
+        <v>0.5824968785696466</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="100" customHeight="1">
+      <c r="A81" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" t="s">
+        <v>165</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>0.58904</v>
+      </c>
+      <c r="F81">
+        <v>2.706709396523279</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="100" customHeight="1">
+      <c r="A82" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82">
+        <v>30.5</v>
+      </c>
+      <c r="E82">
+        <v>0.49352</v>
+      </c>
+      <c r="F82">
+        <v>0.4064631060318465</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="100" customHeight="1">
+      <c r="A83" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83">
         <v>1.5</v>
       </c>
-      <c r="E68">
+      <c r="E83">
         <v>0.58904</v>
       </c>
-      <c r="F68">
+      <c r="F83">
         <v>2.464891741858761</v>
       </c>
     </row>

</xml_diff>